<commit_message>
Mostrar valores na tela 1
Mostrar valores na tela 1.
</commit_message>
<xml_diff>
--- a/Matrizes.xlsx
+++ b/Matrizes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7755"/>
+    <workbookView windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Det" sheetId="1" r:id="rId1"/>
@@ -76,8 +76,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -120,7 +120,46 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -134,8 +173,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -149,7 +212,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -157,7 +220,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -165,22 +228,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -195,69 +257,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -290,49 +290,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -344,127 +452,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -494,21 +494,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -527,18 +512,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -561,7 +550,18 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -570,8 +570,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -598,145 +598,145 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1095,8 +1095,8 @@
   <sheetPr/>
   <dimension ref="A2:W17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
@@ -1117,141 +1117,141 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11">
-      <c r="A2" s="6">
+      <c r="A2" s="1">
         <v>5</v>
       </c>
-      <c r="B2" s="6">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
         <v>5</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="6"/>
+      <c r="J2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="6">
-        <v>3</v>
-      </c>
-      <c r="B3" s="6">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
         <v>4</v>
       </c>
-      <c r="C3" s="6">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6">
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
         <v>6</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6" t="s">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="6"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6">
-        <v>3</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
         <v>6</v>
       </c>
-      <c r="D4" s="6">
-        <v>1</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6" t="s">
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="6"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:23">
-      <c r="A8" s="6">
+      <c r="A8" s="1">
         <f>A2</f>
         <v>5</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="1">
         <f>B2</f>
         <v>1</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="1">
         <f>C2</f>
         <v>1</v>
       </c>
@@ -1263,16 +1263,16 @@
         <f>B8</f>
         <v>1</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="1"/>
       <c r="G8" s="8">
         <f>D2</f>
         <v>5</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="1">
         <f>B2</f>
         <v>1</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="1">
         <f>C2</f>
         <v>1</v>
       </c>
@@ -1284,7 +1284,7 @@
         <f>H8</f>
         <v>1</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="1">
         <f>A2</f>
         <v>5</v>
       </c>
@@ -1292,7 +1292,7 @@
         <f>D2</f>
         <v>5</v>
       </c>
-      <c r="O8" s="6">
+      <c r="O8" s="1">
         <f>C2</f>
         <v>1</v>
       </c>
@@ -1304,11 +1304,11 @@
         <f t="shared" ref="Q8:Q10" si="1">N8</f>
         <v>5</v>
       </c>
-      <c r="S8" s="6">
+      <c r="S8" s="1">
         <f>A2</f>
         <v>5</v>
       </c>
-      <c r="T8" s="6">
+      <c r="T8" s="1">
         <f>B2</f>
         <v>1</v>
       </c>
@@ -1326,15 +1326,15 @@
       </c>
     </row>
     <row r="9" spans="1:23">
-      <c r="A9" s="6">
+      <c r="A9" s="1">
         <f>A3</f>
         <v>3</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="1">
         <f>B3</f>
         <v>4</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="1">
         <f>C3</f>
         <v>1</v>
       </c>
@@ -1346,16 +1346,16 @@
         <f>B9</f>
         <v>4</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="1"/>
       <c r="G9" s="8">
         <f>D3</f>
         <v>6</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="1">
         <f>B3</f>
         <v>4</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="1">
         <f>C3</f>
         <v>1</v>
       </c>
@@ -1367,7 +1367,7 @@
         <f>H9</f>
         <v>4</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="1">
         <f>A3</f>
         <v>3</v>
       </c>
@@ -1375,7 +1375,7 @@
         <f>D3</f>
         <v>6</v>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="1">
         <f>C3</f>
         <v>1</v>
       </c>
@@ -1387,11 +1387,11 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="S9" s="6">
+      <c r="S9" s="1">
         <f>A3</f>
         <v>3</v>
       </c>
-      <c r="T9" s="6">
+      <c r="T9" s="1">
         <f>B3</f>
         <v>4</v>
       </c>
@@ -1409,15 +1409,15 @@
       </c>
     </row>
     <row r="10" spans="1:23">
-      <c r="A10" s="6">
+      <c r="A10" s="1">
         <f>A4</f>
         <v>3</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="1">
         <f>B4</f>
         <v>3</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="1">
         <f>C4</f>
         <v>6</v>
       </c>
@@ -1429,16 +1429,16 @@
         <f>B10</f>
         <v>3</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="1"/>
       <c r="G10" s="8">
         <f>D4</f>
         <v>1</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="1">
         <f>B4</f>
         <v>3</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="1">
         <f>C4</f>
         <v>6</v>
       </c>
@@ -1450,7 +1450,7 @@
         <f>H10</f>
         <v>3</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="1">
         <f>A4</f>
         <v>3</v>
       </c>
@@ -1458,7 +1458,7 @@
         <f>D4</f>
         <v>1</v>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="1">
         <f>C4</f>
         <v>6</v>
       </c>
@@ -1470,11 +1470,11 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="S10" s="6">
+      <c r="S10" s="1">
         <f>A4</f>
         <v>3</v>
       </c>
-      <c r="T10" s="6">
+      <c r="T10" s="1">
         <f>B4</f>
         <v>3</v>
       </c>
@@ -1492,238 +1492,238 @@
       </c>
     </row>
     <row r="11" spans="1:23">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
     </row>
     <row r="12" spans="1:23">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
     </row>
     <row r="13" spans="1:23">
-      <c r="A13" s="6">
+      <c r="A13" s="1">
         <f>$A$8*$B$9*$C$10</f>
         <v>120</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="1">
         <f>$C$8*$B$9*$A$10</f>
         <v>12</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1">
         <f>G8*H9*I10</f>
         <v>120</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="1">
         <f>I8*H9*G10</f>
         <v>4</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="M13" s="6">
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="M13" s="1">
         <f>M8*N9*O10</f>
         <v>180</v>
       </c>
-      <c r="N13" s="6">
+      <c r="N13" s="1">
         <f>O8*N9*M10</f>
         <v>18</v>
       </c>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="S13" s="6">
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="S13" s="1">
         <f>S8*T9*U10</f>
         <v>20</v>
       </c>
-      <c r="T13" s="6">
+      <c r="T13" s="1">
         <f>U8*T9*S10</f>
         <v>60</v>
       </c>
-      <c r="U13" s="6"/>
-      <c r="V13" s="6"/>
-      <c r="W13" s="6"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
     </row>
     <row r="14" spans="1:23">
-      <c r="A14" s="6">
+      <c r="A14" s="1">
         <f>$B$8*$C$9*$D$10</f>
         <v>3</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="1">
         <f>$D$8*$C$9*$B$10</f>
         <v>15</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1">
         <f>H8*I9*J10</f>
         <v>1</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="1">
         <f>J8*I9*H10</f>
         <v>15</v>
       </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="M14" s="6">
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="M14" s="1">
         <f>N8*O9*P10</f>
         <v>15</v>
       </c>
-      <c r="N14" s="6">
+      <c r="N14" s="1">
         <f>P8*O9*N10</f>
         <v>5</v>
       </c>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="S14" s="6">
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="S14" s="1">
         <f>T8*U9*V10</f>
         <v>18</v>
       </c>
-      <c r="T14" s="6">
+      <c r="T14" s="1">
         <f>V8*U9*T10</f>
         <v>90</v>
       </c>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
     </row>
     <row r="15" spans="1:23">
-      <c r="A15" s="6">
+      <c r="A15" s="1">
         <f>$C$8*$D$9*$E$10</f>
         <v>9</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="1">
         <f>$E$8*$D$9*$C$10</f>
         <v>18</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1">
         <f>I8*J9*K10</f>
         <v>18</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="1">
         <f>K8*J9*I10</f>
         <v>36</v>
       </c>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="M15" s="6">
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="M15" s="1">
         <f>O8*P9*Q10</f>
         <v>3</v>
       </c>
-      <c r="N15" s="6">
+      <c r="N15" s="1">
         <f>Q8*P9*O10</f>
         <v>90</v>
       </c>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="S15" s="6">
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="S15" s="1">
         <f>U8*V9*W10</f>
         <v>45</v>
       </c>
-      <c r="T15" s="6">
+      <c r="T15" s="1">
         <f>W8*V9*U10</f>
         <v>3</v>
       </c>
-      <c r="U15" s="6"/>
-      <c r="V15" s="6"/>
-      <c r="W15" s="6"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
     </row>
     <row r="16" spans="1:23">
-      <c r="A16" s="6">
+      <c r="A16" s="1">
         <f>SUM(A13:A15)</f>
         <v>132</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="1">
         <f>SUM(B13:B15)</f>
         <v>45</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1">
         <f>SUM(G13:G15)</f>
         <v>139</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="1">
         <f>SUM(H13:H15)</f>
         <v>55</v>
       </c>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="M16" s="6">
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="M16" s="1">
         <f>SUM(M13:M15)</f>
         <v>198</v>
       </c>
-      <c r="N16" s="6">
+      <c r="N16" s="1">
         <f>SUM(N13:N15)</f>
         <v>113</v>
       </c>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="S16" s="6">
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="S16" s="1">
         <f>SUM(S13:S15)</f>
         <v>83</v>
       </c>
-      <c r="T16" s="6">
+      <c r="T16" s="1">
         <f>SUM(T13:T15)</f>
         <v>153</v>
       </c>
-      <c r="U16" s="6"/>
-      <c r="V16" s="6"/>
-      <c r="W16" s="6"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
     </row>
     <row r="17" spans="1:23">
       <c r="A17" s="9" t="s">
@@ -1733,10 +1733,10 @@
         <f>A16-B16</f>
         <v>87</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
       <c r="G17" s="9" t="s">
         <v>13</v>
       </c>
@@ -1744,9 +1744,9 @@
         <f>G16-H16</f>
         <v>84</v>
       </c>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
       <c r="M17" s="9" t="s">
         <v>13</v>
       </c>
@@ -1754,9 +1754,9 @@
         <f>M16-N16</f>
         <v>85</v>
       </c>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
       <c r="S17" s="9" t="s">
         <v>14</v>
       </c>
@@ -1764,9 +1764,9 @@
         <f>S16-T16</f>
         <v>-70</v>
       </c>
-      <c r="U17" s="6"/>
-      <c r="V17" s="6"/>
-      <c r="W17" s="6"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1777,16 +1777,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="2" width="12.8571428571429" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="12.8571428571429"/>
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="11.7142857142857" customWidth="1"/>
     <col min="7" max="7" width="10.5714285714286" customWidth="1"/>
@@ -2214,6 +2215,119 @@
         <v>0</v>
       </c>
     </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="4">
+        <v>5</v>
+      </c>
+      <c r="B19" s="5">
+        <f>A19*B25</f>
+        <v>4.82758620689655</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5">
+        <f>C19*C25</f>
+        <v>0.977011494252873</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19" s="5">
+        <f>E19*D25</f>
+        <v>-0.804597701149425</v>
+      </c>
+      <c r="G19" s="4">
+        <v>5</v>
+      </c>
+      <c r="H19" s="5">
+        <f t="shared" ref="H19:H21" si="2">ROUND(B19+D19+F19,1)</f>
+        <v>5</v>
+      </c>
+      <c r="I19" s="6">
+        <f t="shared" ref="I19:I21" si="3">B19+D19+F19</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="4">
+        <v>3</v>
+      </c>
+      <c r="B20" s="5">
+        <f>A20*B25</f>
+        <v>2.89655172413793</v>
+      </c>
+      <c r="C20" s="4">
+        <v>4</v>
+      </c>
+      <c r="D20" s="5">
+        <f>C20*C25</f>
+        <v>3.90804597701149</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" s="5">
+        <f>E20*D25</f>
+        <v>-0.804597701149425</v>
+      </c>
+      <c r="G20" s="4">
+        <v>6</v>
+      </c>
+      <c r="H20" s="5">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="I20" s="6">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="4">
+        <v>3</v>
+      </c>
+      <c r="B21" s="5">
+        <f>A21*B25</f>
+        <v>2.89655172413793</v>
+      </c>
+      <c r="C21" s="4">
+        <v>3</v>
+      </c>
+      <c r="D21" s="5">
+        <f>C21*C25</f>
+        <v>2.93103448275862</v>
+      </c>
+      <c r="E21" s="4">
+        <v>6</v>
+      </c>
+      <c r="F21" s="5">
+        <f>E21*D25</f>
+        <v>-4.82758620689655</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
+      </c>
+      <c r="H21" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I21" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25">
+        <v>0.96551724137931</v>
+      </c>
+      <c r="C25">
+        <v>0.977011494252873</v>
+      </c>
+      <c r="D25">
+        <v>-0.804597701149425</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Mostrar valores na tela 2 e Ajuste no critério de parada
Mostrar valores na tela 2 e Ajuste no critério de parada.
</commit_message>
<xml_diff>
--- a/Matrizes.xlsx
+++ b/Matrizes.xlsx
@@ -76,8 +76,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -126,9 +126,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -142,10 +141,40 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -175,37 +204,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -219,23 +233,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -249,15 +256,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -290,37 +290,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -332,139 +464,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,17 +493,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -511,7 +505,48 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -532,41 +567,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -577,16 +577,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -598,149 +598,149 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -757,9 +757,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1255,16 +1252,16 @@
         <f>C2</f>
         <v>1</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <f>A8</f>
         <v>5</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <f>B8</f>
         <v>1</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <f>D2</f>
         <v>5</v>
       </c>
@@ -1276,11 +1273,11 @@
         <f>C2</f>
         <v>1</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="6">
         <f>G8</f>
         <v>5</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="6">
         <f>H8</f>
         <v>1</v>
       </c>
@@ -1288,7 +1285,7 @@
         <f>A2</f>
         <v>5</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="7">
         <f>D2</f>
         <v>5</v>
       </c>
@@ -1296,11 +1293,11 @@
         <f>C2</f>
         <v>1</v>
       </c>
-      <c r="P8" s="7">
+      <c r="P8" s="6">
         <f t="shared" ref="P8:P10" si="0">M8</f>
         <v>5</v>
       </c>
-      <c r="Q8" s="7">
+      <c r="Q8" s="6">
         <f t="shared" ref="Q8:Q10" si="1">N8</f>
         <v>5</v>
       </c>
@@ -1312,15 +1309,15 @@
         <f>B2</f>
         <v>1</v>
       </c>
-      <c r="U8" s="8">
+      <c r="U8" s="7">
         <f>D2</f>
         <v>5</v>
       </c>
-      <c r="V8" s="7">
+      <c r="V8" s="6">
         <f t="shared" ref="V8:V10" si="2">S8</f>
         <v>5</v>
       </c>
-      <c r="W8" s="7">
+      <c r="W8" s="6">
         <f t="shared" ref="W8:W10" si="3">T8</f>
         <v>1</v>
       </c>
@@ -1338,16 +1335,16 @@
         <f>C3</f>
         <v>1</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <f>A9</f>
         <v>3</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <f>B9</f>
         <v>4</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <f>D3</f>
         <v>6</v>
       </c>
@@ -1359,11 +1356,11 @@
         <f>C3</f>
         <v>1</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="6">
         <f>G9</f>
         <v>6</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="6">
         <f>H9</f>
         <v>4</v>
       </c>
@@ -1371,7 +1368,7 @@
         <f>A3</f>
         <v>3</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="7">
         <f>D3</f>
         <v>6</v>
       </c>
@@ -1379,11 +1376,11 @@
         <f>C3</f>
         <v>1</v>
       </c>
-      <c r="P9" s="7">
+      <c r="P9" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="Q9" s="7">
+      <c r="Q9" s="6">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -1395,15 +1392,15 @@
         <f>B3</f>
         <v>4</v>
       </c>
-      <c r="U9" s="8">
+      <c r="U9" s="7">
         <f>D3</f>
         <v>6</v>
       </c>
-      <c r="V9" s="7">
+      <c r="V9" s="6">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="W9" s="7">
+      <c r="W9" s="6">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
@@ -1421,16 +1418,16 @@
         <f>C4</f>
         <v>6</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <f>A10</f>
         <v>3</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <f>B10</f>
         <v>3</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <f>D4</f>
         <v>1</v>
       </c>
@@ -1442,11 +1439,11 @@
         <f>C4</f>
         <v>6</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="6">
         <f>G10</f>
         <v>1</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="6">
         <f>H10</f>
         <v>3</v>
       </c>
@@ -1454,7 +1451,7 @@
         <f>A4</f>
         <v>3</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10" s="7">
         <f>D4</f>
         <v>1</v>
       </c>
@@ -1462,11 +1459,11 @@
         <f>C4</f>
         <v>6</v>
       </c>
-      <c r="P10" s="7">
+      <c r="P10" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="Q10" s="7">
+      <c r="Q10" s="6">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1478,15 +1475,15 @@
         <f>B4</f>
         <v>3</v>
       </c>
-      <c r="U10" s="8">
+      <c r="U10" s="7">
         <f>D4</f>
         <v>1</v>
       </c>
-      <c r="V10" s="7">
+      <c r="V10" s="6">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="W10" s="7">
+      <c r="W10" s="6">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
@@ -1726,10 +1723,10 @@
       <c r="W16" s="1"/>
     </row>
     <row r="17" spans="1:23">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="9">
         <f>A16-B16</f>
         <v>87</v>
       </c>
@@ -1737,30 +1734,30 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H17" s="9">
         <f>G16-H16</f>
         <v>84</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="M17" s="9" t="s">
+      <c r="M17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N17" s="10">
+      <c r="N17" s="9">
         <f>M16-N16</f>
         <v>85</v>
       </c>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-      <c r="S17" s="9" t="s">
+      <c r="S17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="T17" s="10">
+      <c r="T17" s="9">
         <f>S16-T16</f>
         <v>-70</v>
       </c>
@@ -1780,14 +1777,14 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="2" width="12.8571428571429" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="12.8571428571429"/>
+    <col min="4" max="4" width="14"/>
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="11.7142857142857" customWidth="1"/>
     <col min="7" max="7" width="10.5714285714286" customWidth="1"/>
@@ -2215,27 +2212,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:11">
       <c r="A19" s="4">
         <v>5</v>
       </c>
       <c r="B19" s="5">
         <f>A19*B25</f>
-        <v>4.82758620689655</v>
+        <v>-3.33333333333323</v>
       </c>
       <c r="C19" s="4">
         <v>1</v>
       </c>
       <c r="D19" s="5">
         <f>C19*C25</f>
-        <v>0.977011494252873</v>
+        <v>14.6666666666664</v>
       </c>
       <c r="E19" s="4">
         <v>1</v>
       </c>
       <c r="F19" s="5">
         <f>E19*D25</f>
-        <v>-0.804597701149425</v>
+        <v>-6.33333333333325</v>
       </c>
       <c r="G19" s="4">
         <v>5</v>
@@ -2244,32 +2241,35 @@
         <f t="shared" ref="H19:H21" si="2">ROUND(B19+D19+F19,1)</f>
         <v>5</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="1">
         <f t="shared" ref="I19:I21" si="3">B19+D19+F19</f>
+        <v>4.99999999999992</v>
+      </c>
+      <c r="K19">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:11">
       <c r="A20" s="4">
         <v>3</v>
       </c>
       <c r="B20" s="5">
         <f>A20*B25</f>
-        <v>2.89655172413793</v>
+        <v>-1.99999999999994</v>
       </c>
       <c r="C20" s="4">
         <v>4</v>
       </c>
       <c r="D20" s="5">
         <f>C20*C25</f>
-        <v>3.90804597701149</v>
+        <v>58.6666666666656</v>
       </c>
       <c r="E20" s="4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F20" s="5">
         <f>E20*D25</f>
-        <v>-0.804597701149425</v>
+        <v>-50.666666666666</v>
       </c>
       <c r="G20" s="4">
         <v>6</v>
@@ -2278,54 +2278,60 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20" s="1">
         <f t="shared" si="3"/>
+        <v>5.99999999999966</v>
+      </c>
+      <c r="K20">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:11">
       <c r="A21" s="4">
         <v>3</v>
       </c>
       <c r="B21" s="5">
         <f>A21*B25</f>
-        <v>2.89655172413793</v>
+        <v>-1.99999999999994</v>
       </c>
       <c r="C21" s="4">
         <v>3</v>
       </c>
       <c r="D21" s="5">
         <f>C21*C25</f>
-        <v>2.93103448275862</v>
+        <v>43.9999999999992</v>
       </c>
       <c r="E21" s="4">
         <v>6</v>
       </c>
       <c r="F21" s="5">
         <f>E21*D25</f>
-        <v>-4.82758620689655</v>
+        <v>-37.9999999999995</v>
       </c>
       <c r="G21" s="4">
         <v>0</v>
       </c>
       <c r="H21" s="5">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="I21" s="6">
+        <v>4</v>
+      </c>
+      <c r="I21" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3.99999999999976</v>
+      </c>
+      <c r="K21">
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25">
-        <v>0.96551724137931</v>
+        <v>-0.666666666666646</v>
       </c>
       <c r="C25">
-        <v>0.977011494252873</v>
+        <v>14.6666666666664</v>
       </c>
       <c r="D25">
-        <v>-0.804597701149425</v>
+        <v>-6.33333333333325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mostrar valores na tela 3
Mostrar valores na tela 3.
</commit_message>
<xml_diff>
--- a/Matrizes.xlsx
+++ b/Matrizes.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Det" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -78,8 +79,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -120,35 +121,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -170,9 +142,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -194,9 +203,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -219,45 +251,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -290,13 +291,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -308,79 +441,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -393,78 +466,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -489,15 +490,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -541,13 +533,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -571,22 +576,18 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -595,152 +596,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -758,6 +759,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1252,16 +1256,16 @@
         <f>C2</f>
         <v>1</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="7">
         <f>A8</f>
         <v>5</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="7">
         <f>B8</f>
         <v>1</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="7">
+      <c r="G8" s="8">
         <f>D2</f>
         <v>5</v>
       </c>
@@ -1273,11 +1277,11 @@
         <f>C2</f>
         <v>1</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="7">
         <f>G8</f>
         <v>5</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="7">
         <f>H8</f>
         <v>1</v>
       </c>
@@ -1285,7 +1289,7 @@
         <f>A2</f>
         <v>5</v>
       </c>
-      <c r="N8" s="7">
+      <c r="N8" s="8">
         <f>D2</f>
         <v>5</v>
       </c>
@@ -1293,11 +1297,11 @@
         <f>C2</f>
         <v>1</v>
       </c>
-      <c r="P8" s="6">
+      <c r="P8" s="7">
         <f t="shared" ref="P8:P10" si="0">M8</f>
         <v>5</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="Q8" s="7">
         <f t="shared" ref="Q8:Q10" si="1">N8</f>
         <v>5</v>
       </c>
@@ -1309,15 +1313,15 @@
         <f>B2</f>
         <v>1</v>
       </c>
-      <c r="U8" s="7">
+      <c r="U8" s="8">
         <f>D2</f>
         <v>5</v>
       </c>
-      <c r="V8" s="6">
+      <c r="V8" s="7">
         <f t="shared" ref="V8:V10" si="2">S8</f>
         <v>5</v>
       </c>
-      <c r="W8" s="6">
+      <c r="W8" s="7">
         <f t="shared" ref="W8:W10" si="3">T8</f>
         <v>1</v>
       </c>
@@ -1335,16 +1339,16 @@
         <f>C3</f>
         <v>1</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="7">
         <f>A9</f>
         <v>3</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="7">
         <f>B9</f>
         <v>4</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="7">
+      <c r="G9" s="8">
         <f>D3</f>
         <v>6</v>
       </c>
@@ -1356,11 +1360,11 @@
         <f>C3</f>
         <v>1</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="7">
         <f>G9</f>
         <v>6</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="7">
         <f>H9</f>
         <v>4</v>
       </c>
@@ -1368,7 +1372,7 @@
         <f>A3</f>
         <v>3</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N9" s="8">
         <f>D3</f>
         <v>6</v>
       </c>
@@ -1376,11 +1380,11 @@
         <f>C3</f>
         <v>1</v>
       </c>
-      <c r="P9" s="6">
+      <c r="P9" s="7">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="Q9" s="7">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -1392,15 +1396,15 @@
         <f>B3</f>
         <v>4</v>
       </c>
-      <c r="U9" s="7">
+      <c r="U9" s="8">
         <f>D3</f>
         <v>6</v>
       </c>
-      <c r="V9" s="6">
+      <c r="V9" s="7">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="W9" s="6">
+      <c r="W9" s="7">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
@@ -1418,16 +1422,16 @@
         <f>C4</f>
         <v>6</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="7">
         <f>A10</f>
         <v>3</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="7">
         <f>B10</f>
         <v>3</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="7">
+      <c r="G10" s="8">
         <f>D4</f>
         <v>1</v>
       </c>
@@ -1439,11 +1443,11 @@
         <f>C4</f>
         <v>6</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="7">
         <f>G10</f>
         <v>1</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="7">
         <f>H10</f>
         <v>3</v>
       </c>
@@ -1451,7 +1455,7 @@
         <f>A4</f>
         <v>3</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N10" s="8">
         <f>D4</f>
         <v>1</v>
       </c>
@@ -1459,11 +1463,11 @@
         <f>C4</f>
         <v>6</v>
       </c>
-      <c r="P10" s="6">
+      <c r="P10" s="7">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="Q10" s="7">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1475,15 +1479,15 @@
         <f>B4</f>
         <v>3</v>
       </c>
-      <c r="U10" s="7">
+      <c r="U10" s="8">
         <f>D4</f>
         <v>1</v>
       </c>
-      <c r="V10" s="6">
+      <c r="V10" s="7">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="W10" s="6">
+      <c r="W10" s="7">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
@@ -1723,10 +1727,10 @@
       <c r="W16" s="1"/>
     </row>
     <row r="17" spans="1:23">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="10">
         <f>A16-B16</f>
         <v>87</v>
       </c>
@@ -1734,30 +1738,30 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="10">
         <f>G16-H16</f>
         <v>84</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="M17" s="8" t="s">
+      <c r="M17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N17" s="9">
+      <c r="N17" s="10">
         <f>M16-N16</f>
         <v>85</v>
       </c>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-      <c r="S17" s="8" t="s">
+      <c r="S17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="T17" s="9">
+      <c r="T17" s="10">
         <f>S16-T16</f>
         <v>-70</v>
       </c>
@@ -1776,8 +1780,8 @@
   <sheetPr/>
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
@@ -2214,36 +2218,36 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B19" s="5">
         <f>A19*B25</f>
-        <v>-3.33333333333323</v>
+        <v>2.98670694623178e+57</v>
       </c>
       <c r="C19" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" s="5">
         <f>C19*C25</f>
-        <v>14.6666666666664</v>
+        <v>1.99113796415452e+57</v>
       </c>
       <c r="E19" s="4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F19" s="5">
         <f>E19*D25</f>
-        <v>-6.33333333333325</v>
+        <v>3.98227592830904e+57</v>
       </c>
       <c r="G19" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H19" s="5">
         <f t="shared" ref="H19:H21" si="2">ROUND(B19+D19+F19,1)</f>
-        <v>5</v>
+        <v>8.96012083869534e+57</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" ref="I19:I21" si="3">B19+D19+F19</f>
-        <v>4.99999999999992</v>
+        <v>8.96012083869534e+57</v>
       </c>
       <c r="K19">
         <v>5</v>
@@ -2251,36 +2255,36 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B20" s="5">
         <f>A20*B25</f>
-        <v>-1.99999999999994</v>
+        <v>9.9556898207726e+56</v>
       </c>
       <c r="C20" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D20" s="5">
         <f>C20*C25</f>
-        <v>58.6666666666656</v>
+        <v>2.98670694623178e+57</v>
       </c>
       <c r="E20" s="4">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F20" s="5">
         <f>E20*D25</f>
-        <v>-50.666666666666</v>
+        <v>-3.98227592830904e+57</v>
       </c>
       <c r="G20" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H20" s="5">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="3"/>
-        <v>5.99999999999966</v>
+        <v>0</v>
       </c>
       <c r="K20">
         <v>6</v>
@@ -2288,50 +2292,109 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B21" s="5">
         <f>A21*B25</f>
-        <v>-1.99999999999994</v>
+        <v>1.99113796415452e+57</v>
       </c>
       <c r="C21" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21" s="5">
         <f>C21*C25</f>
-        <v>43.9999999999992</v>
+        <v>1.99113796415452e+57</v>
       </c>
       <c r="E21" s="4">
-        <v>6</v>
+        <v>-2</v>
       </c>
       <c r="F21" s="5">
         <f>E21*D25</f>
-        <v>-37.9999999999995</v>
+        <v>7.96455185661808e+57</v>
       </c>
       <c r="G21" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H21" s="5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>1.19468277849271e+58</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" si="3"/>
-        <v>3.99999999999976</v>
+        <v>1.19468277849271e+58</v>
       </c>
       <c r="K21">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:4">
-      <c r="B25">
-        <v>-0.666666666666646</v>
-      </c>
-      <c r="C25">
-        <v>14.6666666666664</v>
-      </c>
-      <c r="D25">
-        <v>-6.33333333333325</v>
+      <c r="B25" s="6">
+        <v>9.9556898207726e+56</v>
+      </c>
+      <c r="C25" s="6">
+        <v>9.9556898207726e+56</v>
+      </c>
+      <c r="D25" s="6">
+        <v>-3.98227592830904e+57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A2:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="3" outlineLevelCol="3"/>
+  <sheetData>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>